<commit_message>
Minor updates and tests
</commit_message>
<xml_diff>
--- a/PIV_Campaign_Processing/Wallcuts.xlsx
+++ b/PIV_Campaign_Processing/Wallcuts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\GitHub\ratzVKI\PIV_Campaign_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324BD15F-7C30-410D-A87A-8493006AAB2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA0E2F7-C980-4AA4-ABF6-63486D1D4EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D1F51DB6-C2AE-454E-B59C-E825C30F28B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1F51DB6-C2AE-454E-B59C-E825C30F28B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,10 +218,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293E4F06-2AD7-43BD-A393-B33F2190FC77}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,16 +549,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
@@ -575,10 +575,10 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
         <v>4</v>
       </c>
       <c r="E3" t="s">
@@ -589,10 +589,10 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>15</v>
       </c>
       <c r="E4" t="s">
@@ -603,10 +603,10 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
         <v>4</v>
       </c>
       <c r="E5" t="s">
@@ -617,10 +617,10 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
         <v>6</v>
       </c>
       <c r="E6" t="s">
@@ -631,10 +631,10 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
       <c r="E7" t="s">
@@ -645,10 +645,10 @@
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E8" t="s">
@@ -659,10 +659,10 @@
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
         <v>9</v>
       </c>
       <c r="E9" t="s">
@@ -673,10 +673,10 @@
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="2">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
         <v>2</v>
       </c>
       <c r="E10" t="s">
@@ -687,10 +687,10 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>-31</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>8</v>
       </c>
       <c r="E11" t="s">
@@ -701,10 +701,10 @@
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
         <v>2</v>
       </c>
       <c r="E12" t="s">
@@ -718,10 +718,10 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>5</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>4</v>
       </c>
       <c r="E13" t="s">
@@ -732,10 +732,10 @@
       <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1">
         <v>3</v>
       </c>
       <c r="E14" t="s">
@@ -746,10 +746,10 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
         <v>3</v>
       </c>
       <c r="E15" t="s">
@@ -760,10 +760,10 @@
       <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="2">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
         <v>3</v>
       </c>
       <c r="E16" t="s">
@@ -774,10 +774,10 @@
       <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="2">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
         <v>3</v>
       </c>
       <c r="E17" t="s">
@@ -788,10 +788,10 @@
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
         <v>2</v>
       </c>
       <c r="E18" t="s">
@@ -802,10 +802,10 @@
       <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>6</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>8</v>
       </c>
       <c r="E19" t="s">
@@ -816,10 +816,10 @@
       <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="2">
-        <v>3</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
         <v>4</v>
       </c>
       <c r="E20" t="s">
@@ -830,10 +830,10 @@
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="2">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="1">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1">
         <v>4</v>
       </c>
       <c r="E21" t="s">
@@ -844,10 +844,10 @@
       <c r="B22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="2">
-        <v>3</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
         <v>3</v>
       </c>
       <c r="E22" t="s">
@@ -858,10 +858,10 @@
       <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="2">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
         <v>3</v>
       </c>
       <c r="E23" t="s">
@@ -872,10 +872,10 @@
       <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>5</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>5</v>
       </c>
       <c r="E24" t="s">
@@ -886,10 +886,10 @@
       <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="2">
-        <v>4</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1">
         <v>4</v>
       </c>
       <c r="E25" t="s">
@@ -900,10 +900,10 @@
       <c r="B26" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="2">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
         <v>4</v>
       </c>
       <c r="E26" t="s">
@@ -914,10 +914,10 @@
       <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="2">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="1">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
         <v>4</v>
       </c>
       <c r="E27" t="s">
@@ -928,10 +928,10 @@
       <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>5</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>5</v>
       </c>
       <c r="E28" t="s">
@@ -942,10 +942,10 @@
       <c r="B29" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>5</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>5</v>
       </c>
       <c r="E29" t="s">
@@ -956,10 +956,10 @@
       <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="2">
-        <v>3</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
         <v>4</v>
       </c>
       <c r="E30" t="s">
@@ -970,10 +970,10 @@
       <c r="B31" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="2">
-        <v>3</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1">
         <v>3</v>
       </c>
       <c r="E31" t="s">
@@ -984,10 +984,10 @@
       <c r="B32" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="2">
-        <v>3</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
         <v>3</v>
       </c>
       <c r="E32" t="s">
@@ -998,10 +998,10 @@
       <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="2">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C33" s="1">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1">
         <v>4</v>
       </c>
       <c r="E33" t="s">
@@ -1012,10 +1012,10 @@
       <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="2">
-        <v>3</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
         <v>4</v>
       </c>
       <c r="E34" t="s">
@@ -1026,10 +1026,10 @@
       <c r="B35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="2">
-        <v>4</v>
-      </c>
-      <c r="D35" s="2">
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
         <v>4</v>
       </c>
       <c r="E35" t="s">
@@ -1040,10 +1040,10 @@
       <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="2">
-        <v>4</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
         <v>4</v>
       </c>
       <c r="E36" t="s">
@@ -1054,10 +1054,10 @@
       <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="2">
-        <v>3</v>
-      </c>
-      <c r="D37" s="2">
+      <c r="C37" s="1">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1">
         <v>3</v>
       </c>
       <c r="E37" t="s">
@@ -1068,10 +1068,10 @@
       <c r="B38" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="2">
-        <v>4</v>
-      </c>
-      <c r="D38" s="2">
+      <c r="C38" s="1">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" t="s">
@@ -1082,10 +1082,10 @@
       <c r="B39" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="2">
-        <v>3</v>
-      </c>
-      <c r="D39" s="2">
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1">
         <v>2</v>
       </c>
       <c r="E39" t="s">

</xml_diff>